<commit_message>
next day test with excel 5 test
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -471,9 +471,55 @@
         <v>2025-06-21T04:13:28.226Z</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>202.173.124.249</v>
+      </c>
+      <c r="B4">
+        <v>28.5212672</v>
+      </c>
+      <c r="C4">
+        <v>77.2243456</v>
+      </c>
+      <c r="D4">
+        <v>735485.4806669627</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Safari/537.36</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Win32</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2025-06-21T04:19:34.989Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>202.173.124.249</v>
+      </c>
+      <c r="B5">
+        <v>28.3621566</v>
+      </c>
+      <c r="C5">
+        <v>77.2827572</v>
+      </c>
+      <c r="D5">
+        <v>15.079999923706055</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2025-06-21T04:20:03.844Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next day test with excel monday test
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -517,9 +517,78 @@
         <v>2025-06-21T04:20:03.844Z</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>202.173.124.249</v>
+      </c>
+      <c r="B6">
+        <v>28.5212672</v>
+      </c>
+      <c r="C6">
+        <v>77.2243456</v>
+      </c>
+      <c r="D6">
+        <v>735485.4806669627</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Safari/537.36</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Win32</v>
+      </c>
+      <c r="G6" t="str">
+        <v>2025-06-21T04:23:56.793Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>106.219.230.230</v>
+      </c>
+      <c r="B7">
+        <v>28.3621629</v>
+      </c>
+      <c r="C7">
+        <v>77.2827333</v>
+      </c>
+      <c r="D7">
+        <v>12.9399995803833</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G7" t="str">
+        <v>2025-06-21T04:24:08.731Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>106.219.230.230</v>
+      </c>
+      <c r="B8">
+        <v>28.3621629</v>
+      </c>
+      <c r="C8">
+        <v>77.2827333</v>
+      </c>
+      <c r="D8">
+        <v>55.656795501708984</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G8" t="str">
+        <v>2025-06-21T04:24:37.801Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next day test with excel wednesday -back camera - drag 3
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -586,9 +586,32 @@
         <v>2025-06-21T04:24:37.801Z</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B9">
+        <v>28.3621642</v>
+      </c>
+      <c r="C9">
+        <v>77.2827832</v>
+      </c>
+      <c r="D9">
+        <v>13.041999816894531</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2025-06-25T16:29:33.084Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next day test with excel wednesday -back camera - drag 4
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -609,9 +609,32 @@
         <v>2025-06-25T16:29:33.084Z</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B10">
+        <v>28.3621531</v>
+      </c>
+      <c r="C10">
+        <v>77.2828514</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2025-06-25T16:37:47.183Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next day test with excel wednesday -back camera - drag 5
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -678,9 +678,32 @@
         <v>2025-06-25T16:50:01.397Z</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B13">
+        <v>28.475392</v>
+      </c>
+      <c r="C13">
+        <v>77.0670592</v>
+      </c>
+      <c r="D13">
+        <v>616570.7228211587</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Safari/537.36</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Win32</v>
+      </c>
+      <c r="G13" t="str">
+        <v>2025-06-25T16:52:19.204Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next day test with excel wednesday -back camera - drag 6
</commit_message>
<xml_diff>
--- a/server/user-data.xlsx
+++ b/server/user-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -701,9 +701,78 @@
         <v>2025-06-25T16:52:19.204Z</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B14">
+        <v>28.3621617</v>
+      </c>
+      <c r="C14">
+        <v>77.2827806</v>
+      </c>
+      <c r="D14">
+        <v>15.01099967956543</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G14" t="str">
+        <v>2025-06-25T17:05:51.318Z</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B15">
+        <v>28.475392</v>
+      </c>
+      <c r="C15">
+        <v>77.0670592</v>
+      </c>
+      <c r="D15">
+        <v>616570.7228211587</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Safari/537.36</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Win32</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2025-06-25T17:05:53.723Z</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>202.173.124.126</v>
+      </c>
+      <c r="B16">
+        <v>28.3621537</v>
+      </c>
+      <c r="C16">
+        <v>77.2828149</v>
+      </c>
+      <c r="D16">
+        <v>12.38599967956543</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/137.0.0.0 Mobile Safari/537.36</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Linux armv81</v>
+      </c>
+      <c r="G16" t="str">
+        <v>2025-06-25T17:07:58.748Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>